<commit_message>
Added event firing class and listners and added code to update excel with customer ID
</commit_message>
<xml_diff>
--- a/src/test/java/com/ibanking/testData/InernetBankingTestData.xlsx
+++ b/src/test/java/com/ibanking/testData/InernetBankingTestData.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amdocs-my.sharepoint.com/personal/nikhilka_amdocs_com/Documents/Backup Folders/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Java_programs\Scratch\src\test\java\com\ibanking\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EF4BC92-02CC-40B1-BC56-AA958C29EBC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6B0BFECC-EAE0-491E-BB80-A5F149CF4B4F}"/>
+    <workbookView windowHeight="7650" windowWidth="16815" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -41,9 +40,6 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>Date of Birth</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -53,29 +49,107 @@
     <t>State</t>
   </si>
   <si>
-    <t>PIN</t>
-  </si>
-  <si>
-    <t>Mobile no.</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
-    <t>Customer ID</t>
+    <t>female</t>
+  </si>
+  <si>
+    <t>DOB(DDMMYYYY)</t>
+  </si>
+  <si>
+    <t>Osfhksg</t>
+  </si>
+  <si>
+    <t>Wsdfimm</t>
+  </si>
+  <si>
+    <t>PIN(6 digit)</t>
+  </si>
+  <si>
+    <t>Mobile no.(10 digit)</t>
+  </si>
+  <si>
+    <t>Email(aa@mail.com format)</t>
+  </si>
+  <si>
+    <t>Customer ID(keep blank)</t>
+  </si>
+  <si>
+    <t>1q2w3e4r</t>
+  </si>
+  <si>
+    <t>Hhhsiuf</t>
+  </si>
+  <si>
+    <t>sif oesifh oi</t>
+  </si>
+  <si>
+    <t>909876</t>
+  </si>
+  <si>
+    <t>kj ajf ih99 kjwd</t>
+  </si>
+  <si>
+    <t>Jlkk</t>
+  </si>
+  <si>
+    <t>887654</t>
+  </si>
+  <si>
+    <t>Row no.</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>15122000</t>
+  </si>
+  <si>
+    <t>qwmnkl</t>
+  </si>
+  <si>
+    <t>8790987656</t>
+  </si>
+  <si>
+    <t>fkjlsf876784@mail.com</t>
+  </si>
+  <si>
+    <t>vnrnvueu bnght</t>
+  </si>
+  <si>
+    <t>22061998</t>
+  </si>
+  <si>
+    <t>9091901128</t>
+  </si>
+  <si>
+    <t>drglkj113350@mail.com</t>
+  </si>
+  <si>
+    <t>42631</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,17 +172,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -125,10 +203,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -163,7 +241,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -215,7 +293,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -326,21 +404,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -357,7 +435,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -409,62 +487,145 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E908422-0353-4DB6-9790-B99A6882E3E5}">
-  <dimension ref="A1:K1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="11" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="7.7109375" collapsed="true"/>
+    <col min="2" max="11" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="23.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="J2"/>
+    <hyperlink r:id="rId2" ref="J3"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added deposit and withdrawfuctionality
</commit_message>
<xml_diff>
--- a/src/test/java/com/ibanking/testData/InernetBankingTestData.xlsx
+++ b/src/test/java/com/ibanking/testData/InernetBankingTestData.xlsx
@@ -1,38 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Java_programs\Scratch\src\test\java\com\ibanking\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr documentId="13_ncr:1_{CDC64972-812C-45C1-B800-AAC25528A128}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView windowHeight="7650" windowWidth="16815" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="NewCustomer" r:id="rId1" sheetId="1"/>
+    <sheet name="NewAccount" r:id="rId2" sheetId="2"/>
+    <sheet name="Deposit" r:id="rId3" sheetId="4"/>
+    <sheet name="Withdrawal" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -109,36 +105,126 @@
     <t>15122000</t>
   </si>
   <si>
-    <t>qwmnkl</t>
-  </si>
-  <si>
-    <t>8790987656</t>
-  </si>
-  <si>
-    <t>fkjlsf876784@mail.com</t>
-  </si>
-  <si>
-    <t>vnrnvueu bnght</t>
-  </si>
-  <si>
     <t>22061998</t>
   </si>
   <si>
-    <t>9091901128</t>
-  </si>
-  <si>
-    <t>drglkj113350@mail.com</t>
-  </si>
-  <si>
-    <t>42631</t>
+    <t>Row  no</t>
+  </si>
+  <si>
+    <t>Customer ID</t>
+  </si>
+  <si>
+    <t>Account Type(Savings/Current)</t>
+  </si>
+  <si>
+    <t>Deposit</t>
+  </si>
+  <si>
+    <t>Account ID (Keep blank)</t>
+  </si>
+  <si>
+    <t>Row no</t>
+  </si>
+  <si>
+    <t>Account no.</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>dflki mmmbk</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>skdn lokn</t>
+  </si>
+  <si>
+    <t>9091901129</t>
+  </si>
+  <si>
+    <t>drglkj113351@mail.com</t>
+  </si>
+  <si>
+    <t>8790987657</t>
+  </si>
+  <si>
+    <t>fkjlsf876785@mail.com</t>
+  </si>
+  <si>
+    <t>90486</t>
+  </si>
+  <si>
+    <t>2227</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>94387</t>
+  </si>
+  <si>
+    <t>94388</t>
+  </si>
+  <si>
+    <t>94389</t>
+  </si>
+  <si>
+    <t>94390</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>Deposit 500</t>
+  </si>
+  <si>
+    <t>Deposit 600</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>2600</t>
+  </si>
+  <si>
+    <t>2300</t>
+  </si>
+  <si>
+    <t>2200</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +236,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,10 +270,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="1"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -494,11 +590,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,40 +605,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -551,13 +647,13 @@
         <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>16</v>
@@ -572,16 +668,16 @@
         <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -589,7 +685,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -610,22 +706,244 @@
         <v>20</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L3"/>
+      <c r="L3" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="J2"/>
-    <hyperlink r:id="rId2" ref="J3"/>
+    <hyperlink r:id="rId1" ref="J2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink r:id="rId2" ref="J3" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8E8576-260C-459B-95A9-69314DF97013}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="13.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="29.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="22.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B087B0-8A77-4C6E-9F2D-ECD9C1763D9C}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="10.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722D8114-E075-4464-B4B2-F4DB4F85257C}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="13.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="13.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>